<commit_message>
create sample data in recommend_data and in ingredents book
</commit_message>
<xml_diff>
--- a/data/recommend_data.xlsx
+++ b/data/recommend_data.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D57C8E-F523-4B49-B3B9-8EA5B7E24260}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="32355" yWindow="2835" windowWidth="9825" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="recomend" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -39,18 +45,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -81,7 +87,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -94,27 +100,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Ingredients"/>
-      <sheetName val="course"/>
-      <sheetName val="元シート"/>
-      <sheetName val="Dummy"/>
-      <sheetName val="lookup"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,18 +364,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.19921875" customWidth="1"/>
-    <col min="3" max="3" width="15.296875" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -401,7 +388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -410,10 +397,10 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(1, 30)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -422,10 +409,10 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C16" ca="1" si="0">RANDBETWEEN(1, 30)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -434,10 +421,10 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -446,10 +433,10 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -458,10 +445,10 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -470,10 +457,10 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -482,10 +469,10 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -494,10 +481,10 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -506,10 +493,10 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -521,7 +508,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -530,10 +517,10 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -542,10 +529,10 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -554,31 +541,31 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>43666</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>43667</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>